<commit_message>
29 sep. data added
</commit_message>
<xml_diff>
--- a/Gold&Lead_TargetCharact_v1.xlsx
+++ b/Gold&Lead_TargetCharact_v1.xlsx
@@ -1,24 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\OneDrive - Universidade de Lisboa\NUCRIA\ISOLDE\Gold_n_Lead\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Alphas" sheetId="1" r:id="rId1"/>
-    <sheet name="Calib 8 ago_v1" sheetId="2" r:id="rId2"/>
+    <sheet name="Alphas" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Calib 8 ago_v1" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="a">Alphas!$M$2</definedName>
+    <definedName function="false" hidden="false" name="a" vbProcedure="false">Alphas!$M$2</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -30,37 +26,37 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="108">
   <si>
-    <t>Nuclide</t>
-  </si>
-  <si>
-    <t>E alpha (keV)</t>
-  </si>
-  <si>
-    <t>Branch (%)</t>
-  </si>
-  <si>
-    <t>T 1/2</t>
-  </si>
-  <si>
-    <t>T 1/2 (s)</t>
-  </si>
-  <si>
-    <t>Alphas from 232U (68.9 y 4)</t>
-  </si>
-  <si>
-    <t>Alphas from 228Th (1.9116 y 16)</t>
-  </si>
-  <si>
-    <t>Alphas from 224Ra (3.66 d 4)</t>
-  </si>
-  <si>
-    <t>Alphas from 220Rn (55.6 s 1)</t>
-  </si>
-  <si>
-    <t>232U</t>
-  </si>
-  <si>
-    <t>68,9 y</t>
+    <t xml:space="preserve">Nuclide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E alpha (keV)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branch (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T 1/2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T 1/2 (s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alphas from 232U (68.9 y 4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alphas from 228Th (1.9116 y 16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alphas from 224Ra (3.66 d 4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alphas from 220Rn (55.6 s 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">232U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68,9 y</t>
   </si>
   <si>
     <t xml:space="preserve">Ea (keV)     </t>
@@ -69,7 +65,7 @@
     <t xml:space="preserve">Ia (%)    </t>
   </si>
   <si>
-    <t>Ia (%)</t>
+    <t xml:space="preserve">Ia (%)</t>
   </si>
   <si>
     <t xml:space="preserve">4460.94(calc)  </t>
@@ -87,10 +83,10 @@
     <t xml:space="preserve">0.114 17 </t>
   </si>
   <si>
-    <t>228Th</t>
-  </si>
-  <si>
-    <t>1,9116 y</t>
+    <t xml:space="preserve">228Th</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,9116 y</t>
   </si>
   <si>
     <t xml:space="preserve">4502.80(calc)  </t>
@@ -108,7 +104,7 @@
     <t xml:space="preserve">6288.08 10  </t>
   </si>
   <si>
-    <t>99.886 17</t>
+    <t xml:space="preserve">99.886 17</t>
   </si>
   <si>
     <t xml:space="preserve">4810.04(calc)  </t>
@@ -123,10 +119,10 @@
     <t xml:space="preserve">0.0073 </t>
   </si>
   <si>
-    <t>224Ra</t>
-  </si>
-  <si>
-    <t>3,66 d</t>
+    <t xml:space="preserve">224Ra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,66 d</t>
   </si>
   <si>
     <t xml:space="preserve">4931.04(calc)  </t>
@@ -156,7 +152,7 @@
     <t xml:space="preserve">5423.15 22  </t>
   </si>
   <si>
-    <t>72.2 11</t>
+    <t xml:space="preserve">72.2 11</t>
   </si>
   <si>
     <t xml:space="preserve">5685.37 15  </t>
@@ -165,10 +161,10 @@
     <t xml:space="preserve">94.92 4 </t>
   </si>
   <si>
-    <t>220Rn</t>
-  </si>
-  <si>
-    <t>55,6 s</t>
+    <t xml:space="preserve">220Rn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55,6 s</t>
   </si>
   <si>
     <t xml:space="preserve">4997.94(calc)  </t>
@@ -177,10 +173,10 @@
     <t xml:space="preserve">0.00616 8 </t>
   </si>
   <si>
-    <t>216Po</t>
-  </si>
-  <si>
-    <t>0,145 s</t>
+    <t xml:space="preserve">216Po</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,145 s</t>
   </si>
   <si>
     <t xml:space="preserve">5139.0 20  </t>
@@ -189,10 +185,10 @@
     <t xml:space="preserve">0.30 2 </t>
   </si>
   <si>
-    <t>212Bi</t>
-  </si>
-  <si>
-    <t>60,55 m</t>
+    <t xml:space="preserve">212Bi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60,55 m</t>
   </si>
   <si>
     <t xml:space="preserve">5263.36 9  </t>
@@ -207,19 +203,19 @@
     <t xml:space="preserve">68.15 23 </t>
   </si>
   <si>
-    <t>Alphas from 216Po (0.145 s 2)</t>
-  </si>
-  <si>
-    <t>Alphas from 212Bi (60.55 m 6)</t>
-  </si>
-  <si>
-    <t>Alphas from 212Po (0.299 us 2)</t>
-  </si>
-  <si>
-    <t>212Po</t>
-  </si>
-  <si>
-    <t>0,299 us</t>
+    <t xml:space="preserve">Alphas from 216Po (0.145 s 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alphas from 212Bi (60.55 m 6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alphas from 212Po (0.299 us 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">212Po</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,299 us</t>
   </si>
   <si>
     <t xml:space="preserve">0.0019 3 </t>
@@ -237,7 +233,7 @@
     <t xml:space="preserve">6778.3 5  </t>
   </si>
   <si>
-    <t>99.9981 3</t>
+    <t xml:space="preserve">99.9981 3</t>
   </si>
   <si>
     <t xml:space="preserve">0.001 </t>
@@ -255,7 +251,7 @@
     <t xml:space="preserve">1.78 </t>
   </si>
   <si>
-    <t>Bi alfa mean energy</t>
+    <t xml:space="preserve">Bi alfa mean energy</t>
   </si>
   <si>
     <t xml:space="preserve">6050.78 3  </t>
@@ -264,13 +260,13 @@
     <t xml:space="preserve">69.91 15 </t>
   </si>
   <si>
-    <t>(keV)</t>
-  </si>
-  <si>
-    <t>Intensity (%)</t>
-  </si>
-  <si>
-    <t>Norm. Intensity (%)</t>
+    <t xml:space="preserve">(keV)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intensity (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norm. Intensity (%)</t>
   </si>
   <si>
     <t xml:space="preserve">6089.88 3  </t>
@@ -279,99 +275,117 @@
     <t xml:space="preserve">27.12 14 </t>
   </si>
   <si>
-    <t># peak</t>
-  </si>
-  <si>
-    <t>ROI Down</t>
-  </si>
-  <si>
-    <t>ROI Up</t>
-  </si>
-  <si>
-    <t>Total integral</t>
-  </si>
-  <si>
-    <t>Net Integral</t>
-  </si>
-  <si>
-    <t>Centroid</t>
-  </si>
-  <si>
-    <t>Max.</t>
-  </si>
-  <si>
-    <t>Sigma</t>
-  </si>
-  <si>
-    <t>FWHM</t>
-  </si>
-  <si>
-    <t>Sigma (keV)</t>
-  </si>
-  <si>
-    <t>E alpha calib (keV)</t>
-  </si>
-  <si>
-    <t>E calib 2 (keV)</t>
-  </si>
-  <si>
-    <t>dEcalib2 (keV)</t>
-  </si>
-  <si>
-    <t>E (keV) =</t>
-  </si>
-  <si>
-    <t>* Channel +</t>
-  </si>
-  <si>
-    <t>Com incertezas nos canais</t>
-  </si>
-  <si>
-    <t>Calib 2</t>
-  </si>
-  <si>
-    <t>TIME OF</t>
-  </si>
-  <si>
-    <t>AQUI.</t>
-  </si>
-  <si>
-    <t>10028 s</t>
-  </si>
-  <si>
-    <t>+-</t>
-  </si>
-  <si>
-    <t>Sigma/E =</t>
-  </si>
-  <si>
-    <t>* 1/sqrt€ +</t>
-  </si>
-  <si>
-    <t>R = sigma/E (MeV)</t>
-  </si>
-  <si>
-    <t>1/sqrt(E) (MeV)</t>
+    <t xml:space="preserve"># peak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROI Down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROI Up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total integral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net Integral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centroid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sigma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FWHM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sigma (keV)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E alpha calib (keV)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E calib 2 (keV)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dEcalib2 (keV)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R = sigma/E (MeV)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/sqrt(E) (MeV)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E (keV) =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Channel +</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Com incertezas nos canais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calib 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIME OF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AQUI.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10028 s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sigma/E =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* 1/sqrtE’+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="0.000E+00"/>
-    <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0000000"/>
-    <numFmt numFmtId="168" formatCode="0.000000"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="8">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.000E+00"/>
+    <numFmt numFmtId="166" formatCode="General"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.00"/>
+    <numFmt numFmtId="170" formatCode="0.0000000"/>
+    <numFmt numFmtId="171" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -381,7 +395,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -389,7 +403,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -410,12 +424,36 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
+      <u val="single"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF595959"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF595959"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF595959"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="23">
@@ -482,7 +520,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFDBB6"/>
-        <bgColor rgb="FFFBE5D6"/>
+        <bgColor rgb="FFFFE994"/>
       </patternFill>
     </fill>
     <fill>
@@ -553,346 +591,421 @@
     </fill>
   </fills>
   <borders count="13">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
       <right/>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
+      <top style="hair"/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
+      <right style="medium"/>
+      <top style="hair"/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
+      <top style="hair"/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
+      <right style="hair"/>
+      <top style="hair"/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
+      <right style="medium"/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
+      <right style="hair"/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
       <right/>
       <top/>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
+      <right style="medium"/>
       <top/>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
+      <right style="hair"/>
       <top/>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="72">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="12" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="13" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="16" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="17" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="18" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="19" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="20" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="22" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="22" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="21" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="22" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -906,11 +1019,11 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFFF5CE"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFBFBFBF"/>
-      <rgbColor rgb="FFFFF2CC"/>
+      <rgbColor rgb="FFFFF5CE"/>
       <rgbColor rgb="FF5B9BD5"/>
       <rgbColor rgb="FFF03E75"/>
       <rgbColor rgb="FFFFFFD7"/>
@@ -933,7 +1046,7 @@
       <rgbColor rgb="FFFFFFA6"/>
       <rgbColor rgb="FFA9D18E"/>
       <rgbColor rgb="FFF8A6BF"/>
-      <rgbColor rgb="FFFBE5D6"/>
+      <rgbColor rgb="FFFFF2CC"/>
       <rgbColor rgb="FFFFDBB6"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF3DEB3D"/>
@@ -944,40 +1057,22 @@
       <rgbColor rgb="FF595959"/>
       <rgbColor rgb="FFBF819E"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF70AD47"/>
+      <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -986,7 +1081,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="pt-PT" sz="1400" b="0" strike="noStrike" spc="-1">
+              <a:defRPr b="0" lang="pt-PT" sz="1400" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -994,7 +1089,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="pt-PT" sz="1400" b="0" strike="noStrike" spc="-1">
+              <a:rPr b="0" lang="pt-PT" sz="1400" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1005,7 +1100,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1016,7 +1110,6 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -1024,9 +1117,20 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Calibration E vs Ch</c:v>
+            <c:strRef>
+              <c:f>"Calibration E vs Ch"</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Calibration E vs Ch</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
             <a:ln w="25560">
               <a:noFill/>
             </a:ln>
@@ -1036,31 +1140,23 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="5B9BD5"/>
+                <a:srgbClr val="5b9bd5"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="pt-PT"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -1069,32 +1165,24 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
           </c:dLbls>
           <c:trendline>
             <c:spPr>
-              <a:ln w="19080" cap="rnd">
+              <a:ln cap="rnd" w="19080">
                 <a:solidFill>
-                  <a:srgbClr val="5B9BD5"/>
+                  <a:srgbClr val="5b9bd5"/>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
                 <a:round/>
               </a:ln>
             </c:spPr>
             <c:trendlineType val="linear"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1127,7 +1215,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>8784.3700000000008</c:v>
+                  <c:v>8784.37</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6778.3</c:v>
@@ -1135,8 +1223,8 @@
                 <c:pt idx="2">
                   <c:v>6288.08</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0.00">
-                  <c:v>6061.7084963413399</c:v>
+                <c:pt idx="3">
+                  <c:v>6061.70849634134</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5685.37</c:v>
@@ -1146,19 +1234,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1580129360"/>
-        <c:axId val="1580129904"/>
+        <c:axId val="97674700"/>
+        <c:axId val="26992949"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1580129360"/>
+        <c:axId val="97674700"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1168,7 +1248,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="D9D9D9"/>
+                <a:srgbClr val="d9d9d9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1181,7 +1261,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="pt-PT" sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr b="0" lang="pt-PT" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1189,7 +1269,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pt-PT" sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:rPr b="0" lang="pt-PT" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1200,7 +1280,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1216,7 +1295,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="BFBFBF"/>
+              <a:srgbClr val="bfbfbf"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1226,22 +1305,21 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1580129904"/>
+        <c:crossAx val="26992949"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1580129904"/>
+        <c:axId val="26992949"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1251,7 +1329,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="D9D9D9"/>
+                <a:srgbClr val="d9d9d9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1264,7 +1342,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="pt-PT" sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr b="0" lang="pt-PT" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1272,7 +1350,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pt-PT" sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:rPr b="0" lang="pt-PT" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1283,7 +1361,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1299,7 +1376,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="BFBFBF"/>
+              <a:srgbClr val="bfbfbf"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1309,17 +1386,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1580129360"/>
+        <c:crossAx val="97674700"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1332,33 +1408,25 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
+      <a:srgbClr val="ffffff"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="D9D9D9"/>
+        <a:srgbClr val="d9d9d9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1367,7 +1435,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="pt-PT" sz="1400" b="0" strike="noStrike" spc="-1">
+              <a:defRPr b="0" lang="pt-PT" sz="1400" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1375,7 +1443,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="pt-PT" sz="1400" b="0" strike="noStrike" spc="-1">
+              <a:rPr b="0" lang="pt-PT" sz="1400" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1386,7 +1454,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1397,7 +1464,6 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -1405,6 +1471,9 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
             <a:ln w="19080">
               <a:noFill/>
             </a:ln>
@@ -1414,31 +1483,37 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="5B9BD5"/>
+                <a:srgbClr val="5b9bd5"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:dPt>
             <c:idx val="4"/>
-            <c:bubble3D val="0"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="5b9bd5"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="4"/>
-              <c:spPr/>
               <c:txPr>
                 <a:bodyPr/>
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
                       <a:solidFill>
                         <a:srgbClr val="000000"/>
                       </a:solidFill>
                       <a:latin typeface="Calibri"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pt-PT"/>
                 </a:p>
               </c:txPr>
               <c:dLblPos val="r"/>
@@ -1447,28 +1522,20 @@
               <c:showCatName val="0"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
-              <c:showBubbleSize val="1"/>
+              <c:separator>; </c:separator>
             </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="pt-PT"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -1477,53 +1544,45 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
           </c:dLbls>
           <c:trendline>
             <c:spPr>
-              <a:ln w="19080" cap="rnd">
+              <a:ln cap="rnd" w="19080">
                 <a:solidFill>
-                  <a:srgbClr val="5B9BD5"/>
+                  <a:srgbClr val="5b9bd5"/>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
                 <a:round/>
               </a:ln>
             </c:spPr>
             <c:trendlineType val="linear"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Calib 8 ago_v1'!$T$2:$T$6</c:f>
               <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.33739969833423611</c:v>
+                  <c:v>0.337399698334236</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.38409584294877042</c:v>
+                  <c:v>0.38409584294877</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.39878698020940273</c:v>
+                  <c:v>0.398786980209403</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.40616498082144353</c:v>
+                  <c:v>0.406164980821444</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.41939247443586286</c:v>
+                  <c:v>0.419392474435863</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1532,41 +1591,33 @@
             <c:numRef>
               <c:f>'Calib 8 ago_v1'!$S$2:$S$6</c:f>
               <c:numCache>
-                <c:formatCode>0.0000000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3.1225733888713704E-3</c:v>
+                  <c:v>0.00312257338887137</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.7740642934069018E-3</c:v>
+                  <c:v>0.0047740642934069</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.2175290390707504E-3</c:v>
+                  <c:v>0.00521752903907075</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.8947982269204144E-3</c:v>
+                  <c:v>0.00489479822692041</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.7627595037789969E-3</c:v>
+                  <c:v>0.005762759503779</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1580128272"/>
-        <c:axId val="1580136976"/>
+        <c:axId val="89278394"/>
+        <c:axId val="42613255"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1580128272"/>
+        <c:axId val="89278394"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1576,7 +1627,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="D9D9D9"/>
+                <a:srgbClr val="d9d9d9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1589,7 +1640,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="pt-PT" sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr b="0" lang="pt-PT" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1597,7 +1648,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pt-PT" sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:rPr b="0" lang="pt-PT" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1608,7 +1659,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1624,7 +1674,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="BFBFBF"/>
+              <a:srgbClr val="bfbfbf"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1634,22 +1684,21 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1580136976"/>
+        <c:crossAx val="42613255"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1580136976"/>
+        <c:axId val="42613255"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1659,7 +1708,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="D9D9D9"/>
+                <a:srgbClr val="d9d9d9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1672,7 +1721,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="pt-PT" sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr b="0" lang="pt-PT" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1680,7 +1729,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pt-PT" sz="1000" b="0" strike="noStrike" spc="-1">
+                  <a:rPr b="0" lang="pt-PT" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1691,7 +1740,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1707,7 +1755,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="BFBFBF"/>
+              <a:srgbClr val="bfbfbf"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1717,17 +1765,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1580128272"/>
+        <c:crossAx val="89278394"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1740,29 +1787,23 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
+      <a:srgbClr val="ffffff"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="D9D9D9"/>
+        <a:srgbClr val="d9d9d9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1772,23 +1813,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>71640</xdr:colOff>
+      <xdr:colOff>71280</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>30960</xdr:rowOff>
+      <xdr:rowOff>30600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1"/>
+        <xdr:cNvPr id="0" name="Image 1" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip r:embed="rId1"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="105480" y="82080"/>
-          <a:ext cx="2691360" cy="3835080"/>
+          <a:ext cx="2696040" cy="3447360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1804,7 +1845,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1814,18 +1855,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>212040</xdr:colOff>
+      <xdr:colOff>211680</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>68760</xdr:rowOff>
+      <xdr:rowOff>68400</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
+    <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="1" name="Gráfico 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off x="518400" y="2328120"/>
+        <a:ext cx="5154120" cy="2750400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1844,18 +1885,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>204120</xdr:colOff>
+      <xdr:colOff>203760</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>89280</xdr:rowOff>
+      <xdr:rowOff>88920</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
+    <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvPr id="2" name="Gráfico 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off x="10269720" y="1967760"/>
+        <a:ext cx="6966360" cy="2578680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1873,24 +1914,24 @@
       <xdr:rowOff>41400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>70</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>682200</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>141840</xdr:rowOff>
+      <xdr:rowOff>141480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Image 2"/>
+        <xdr:cNvPr id="3" name="Image 2" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip r:embed="rId3"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="497160" y="5335920"/>
-          <a:ext cx="5607720" cy="3967560"/>
+          <a:off x="497160" y="5235480"/>
+          <a:ext cx="5645880" cy="3967200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1905,305 +1946,47 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="F1:W27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="5" max="5" width="3.6328125" customWidth="1"/>
-    <col min="6" max="6" width="11.54296875" customWidth="1"/>
-    <col min="10" max="12" width="10.1796875" customWidth="1"/>
-    <col min="13" max="13" width="15.81640625" customWidth="1"/>
-    <col min="14" max="14" width="10.1796875" customWidth="1"/>
-    <col min="15" max="15" width="17.1796875" customWidth="1"/>
-    <col min="16" max="16" width="10.1796875" customWidth="1"/>
-    <col min="17" max="17" width="17" customWidth="1"/>
-    <col min="18" max="18" width="10.08984375" customWidth="1"/>
-    <col min="19" max="19" width="15.1796875" customWidth="1"/>
-    <col min="20" max="20" width="10.1796875" customWidth="1"/>
-    <col min="21" max="21" width="10.90625" customWidth="1"/>
-    <col min="22" max="22" width="15.90625" customWidth="1"/>
-    <col min="23" max="23" width="10.08984375" customWidth="1"/>
-    <col min="24" max="24" width="17.26953125" customWidth="1"/>
-    <col min="25" max="25" width="10.54296875" customWidth="1"/>
-    <col min="26" max="26" width="17.1796875" customWidth="1"/>
-    <col min="28" max="28" width="2.453125" customWidth="1"/>
-    <col min="29" max="29" width="10.90625" customWidth="1"/>
-    <col min="30" max="30" width="9.08984375" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="3.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="10.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="10.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="10.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="10.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="10.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="15.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="10.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="17.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="10.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="17.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="2.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="10.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="9.09"/>
   </cols>
   <sheetData>
-    <row r="1" spans="8:23" x14ac:dyDescent="0.35">
+    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
     </row>
-    <row r="2" spans="8:23" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2236,21 +2019,21 @@
       </c>
       <c r="T2" s="7"/>
     </row>
-    <row r="3" spans="8:23" x14ac:dyDescent="0.35">
+    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="9" t="n">
         <v>5320.12</v>
       </c>
-      <c r="J3" s="10">
-        <v>68.150000000000006</v>
+      <c r="J3" s="10" t="n">
+        <v>68.15</v>
       </c>
       <c r="K3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="12">
-        <f>68.9*365.25*24*3600</f>
+      <c r="L3" s="12" t="n">
+        <f aca="false">68.9*365.25*24*3600</f>
         <v>2174318640</v>
       </c>
       <c r="M3" s="13" t="s">
@@ -2278,12 +2061,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="8:23" x14ac:dyDescent="0.35">
+    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H4" s="8"/>
-      <c r="I4" s="9">
+      <c r="I4" s="9" t="n">
         <v>5263.36</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="10" t="n">
         <v>31.55</v>
       </c>
       <c r="K4" s="17"/>
@@ -2294,41 +2077,41 @@
       <c r="N4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="O4" s="14">
+      <c r="O4" s="14" t="n">
         <v>5138</v>
       </c>
       <c r="P4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" s="15">
+      <c r="Q4" s="15" t="n">
         <v>5034</v>
       </c>
       <c r="R4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="S4" s="16">
+      <c r="S4" s="16" t="n">
         <v>5747</v>
       </c>
       <c r="T4" s="16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="8:23" x14ac:dyDescent="0.35">
+    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="9" t="n">
         <v>5423.15</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="10" t="n">
         <v>72.2</v>
       </c>
       <c r="K5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="12">
-        <f>1.9116*365.25*24*3600</f>
-        <v>60325508.159999996</v>
+      <c r="L5" s="12" t="n">
+        <f aca="false">1.9116*365.25*24*3600</f>
+        <v>60325508.16</v>
       </c>
       <c r="M5" s="13" t="s">
         <v>21</v>
@@ -2336,13 +2119,13 @@
       <c r="N5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="14">
+      <c r="O5" s="14" t="n">
         <v>5173</v>
       </c>
       <c r="P5" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Q5" s="15">
+      <c r="Q5" s="15" t="n">
         <v>5051</v>
       </c>
       <c r="R5" s="15" t="s">
@@ -2355,12 +2138,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="8:23" x14ac:dyDescent="0.35">
+    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H6" s="8"/>
-      <c r="I6" s="9">
+      <c r="I6" s="9" t="n">
         <v>5340.36</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="10" t="n">
         <v>27.2</v>
       </c>
       <c r="K6" s="11"/>
@@ -2371,13 +2154,13 @@
       <c r="N6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="O6" s="14">
+      <c r="O6" s="14" t="n">
         <v>5211</v>
       </c>
       <c r="P6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="Q6" s="15">
+      <c r="Q6" s="15" t="n">
         <v>5161</v>
       </c>
       <c r="R6" s="15" t="s">
@@ -2386,21 +2169,21 @@
       <c r="S6" s="16"/>
       <c r="T6" s="16"/>
     </row>
-    <row r="7" spans="8:23" x14ac:dyDescent="0.35">
+    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H7" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="9" t="n">
         <v>5685.37</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="10" t="n">
         <v>94.92</v>
       </c>
       <c r="K7" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="L7" s="20">
-        <f>3.66*24*3600</f>
+      <c r="L7" s="20" t="n">
+        <f aca="false">3.66*24*3600</f>
         <v>316224</v>
       </c>
       <c r="M7" s="13" t="s">
@@ -2424,13 +2207,13 @@
       <c r="S7" s="16"/>
       <c r="T7" s="16"/>
     </row>
-    <row r="8" spans="8:23" x14ac:dyDescent="0.35">
+    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H8" s="23"/>
-      <c r="I8" s="24">
+      <c r="I8" s="24" t="n">
         <v>5448.6</v>
       </c>
-      <c r="J8" s="25">
-        <v>5.0599999999999996</v>
+      <c r="J8" s="25" t="n">
+        <v>5.06</v>
       </c>
       <c r="K8" s="26"/>
       <c r="L8" s="27"/>
@@ -2455,21 +2238,21 @@
       <c r="S8" s="16"/>
       <c r="T8" s="16"/>
     </row>
-    <row r="9" spans="8:23" x14ac:dyDescent="0.35">
+    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H9" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="9" t="n">
         <v>6288.08</v>
       </c>
-      <c r="J9" s="10">
-        <v>99.885999999999996</v>
+      <c r="J9" s="10" t="n">
+        <v>99.886</v>
       </c>
       <c r="K9" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="L9" s="12">
-        <f>55.6</f>
+      <c r="L9" s="12" t="n">
+        <f aca="false">55.6</f>
         <v>55.6</v>
       </c>
       <c r="M9" s="13" t="s">
@@ -2485,22 +2268,22 @@
       <c r="S9" s="16"/>
       <c r="T9" s="16"/>
     </row>
-    <row r="10" spans="8:23" x14ac:dyDescent="0.35">
+    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H10" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="9" t="n">
         <v>6778.3</v>
       </c>
-      <c r="J10" s="10">
-        <v>99.998099999999994</v>
+      <c r="J10" s="10" t="n">
+        <v>99.9981</v>
       </c>
       <c r="K10" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="L10" s="18">
-        <f>0.145</f>
-        <v>0.14499999999999999</v>
+      <c r="L10" s="18" t="n">
+        <f aca="false">0.145</f>
+        <v>0.145</v>
       </c>
       <c r="M10" s="13" t="s">
         <v>51</v>
@@ -2515,21 +2298,21 @@
       <c r="S10" s="16"/>
       <c r="T10" s="16"/>
     </row>
-    <row r="11" spans="8:23" x14ac:dyDescent="0.35">
+    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H11" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="9" t="n">
         <v>6050.78</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="10" t="n">
         <v>69.91</v>
       </c>
       <c r="K11" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="L11" s="12">
-        <f>60.55*365.25/12*24*3600</f>
+      <c r="L11" s="12" t="n">
+        <f aca="false">60.55*365.25/12*24*3600</f>
         <v>159234390</v>
       </c>
       <c r="M11" s="28" t="s">
@@ -2545,12 +2328,12 @@
       <c r="S11" s="16"/>
       <c r="T11" s="16"/>
     </row>
-    <row r="12" spans="8:23" x14ac:dyDescent="0.35">
+    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H12" s="8"/>
-      <c r="I12" s="9">
+      <c r="I12" s="9" t="n">
         <v>6089.88</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="10" t="n">
         <v>27.12</v>
       </c>
       <c r="K12" s="11"/>
@@ -2568,23 +2351,23 @@
       <c r="S12" s="16"/>
       <c r="T12" s="16"/>
     </row>
-    <row r="13" spans="8:23" x14ac:dyDescent="0.35">
+    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H13" s="8"/>
-      <c r="I13" s="9">
+      <c r="I13" s="9" t="n">
         <v>5768</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="10" t="n">
         <v>1.78</v>
       </c>
       <c r="K13" s="11"/>
       <c r="L13" s="20"/>
     </row>
-    <row r="14" spans="8:23" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H14" s="23"/>
-      <c r="I14" s="24">
+      <c r="I14" s="24" t="n">
         <v>5607</v>
       </c>
-      <c r="J14" s="25">
+      <c r="J14" s="25" t="n">
         <v>1.19</v>
       </c>
       <c r="K14" s="26"/>
@@ -2602,22 +2385,22 @@
       </c>
       <c r="R14" s="7"/>
     </row>
-    <row r="15" spans="8:23" x14ac:dyDescent="0.35">
+    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H15" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="I15" s="9">
-        <v>8784.3700000000008</v>
-      </c>
-      <c r="J15" s="10">
+      <c r="I15" s="9" t="n">
+        <v>8784.37</v>
+      </c>
+      <c r="J15" s="10" t="n">
         <v>100</v>
       </c>
       <c r="K15" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="L15" s="12">
-        <f>0.000000299</f>
-        <v>2.9900000000000002E-7</v>
+      <c r="L15" s="12" t="n">
+        <f aca="false">0.000000299</f>
+        <v>2.99E-007</v>
       </c>
       <c r="M15" s="29" t="s">
         <v>11</v>
@@ -2638,13 +2421,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="8:23" x14ac:dyDescent="0.35">
+    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H16" s="8"/>
       <c r="I16" s="9"/>
       <c r="J16" s="10"/>
       <c r="K16" s="17"/>
       <c r="L16" s="18"/>
-      <c r="M16" s="29">
+      <c r="M16" s="29" t="n">
         <v>5985</v>
       </c>
       <c r="N16" s="29" t="s">
@@ -2659,11 +2442,11 @@
       <c r="Q16" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="R16" s="32">
+      <c r="R16" s="32" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="6:18" x14ac:dyDescent="0.35">
+    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H17" s="8"/>
       <c r="I17" s="9"/>
       <c r="J17" s="10"/>
@@ -2675,7 +2458,7 @@
       <c r="N17" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="O17" s="30">
+      <c r="O17" s="30" t="n">
         <v>5345</v>
       </c>
       <c r="P17" s="30" t="s">
@@ -2684,7 +2467,7 @@
       <c r="Q17" s="31"/>
       <c r="R17" s="31"/>
     </row>
-    <row r="18" spans="6:18" x14ac:dyDescent="0.35">
+    <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H18" s="8"/>
       <c r="I18" s="9"/>
       <c r="J18" s="10"/>
@@ -2692,7 +2475,7 @@
       <c r="L18" s="20"/>
       <c r="M18" s="29"/>
       <c r="N18" s="29"/>
-      <c r="O18" s="30">
+      <c r="O18" s="30" t="n">
         <v>5481</v>
       </c>
       <c r="P18" s="30" t="s">
@@ -2701,7 +2484,7 @@
       <c r="Q18" s="31"/>
       <c r="R18" s="31"/>
     </row>
-    <row r="19" spans="6:18" x14ac:dyDescent="0.35">
+    <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H19" s="8"/>
       <c r="I19" s="9"/>
       <c r="J19" s="10"/>
@@ -2709,7 +2492,7 @@
       <c r="L19" s="20"/>
       <c r="M19" s="29"/>
       <c r="N19" s="29"/>
-      <c r="O19" s="34">
+      <c r="O19" s="34" t="n">
         <v>5607</v>
       </c>
       <c r="P19" s="34" t="s">
@@ -2718,10 +2501,10 @@
       <c r="Q19" s="31"/>
       <c r="R19" s="31"/>
     </row>
-    <row r="20" spans="6:18" x14ac:dyDescent="0.35">
+    <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M20" s="29"/>
       <c r="N20" s="29"/>
-      <c r="O20" s="30">
+      <c r="O20" s="30" t="n">
         <v>5626</v>
       </c>
       <c r="P20" s="30" t="s">
@@ -2730,10 +2513,10 @@
       <c r="Q20" s="31"/>
       <c r="R20" s="31"/>
     </row>
-    <row r="21" spans="6:18" x14ac:dyDescent="0.35">
+    <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M21" s="29"/>
       <c r="N21" s="29"/>
-      <c r="O21" s="34">
+      <c r="O21" s="34" t="n">
         <v>5768</v>
       </c>
       <c r="P21" s="34" t="s">
@@ -2742,7 +2525,7 @@
       <c r="Q21" s="31"/>
       <c r="R21" s="31"/>
     </row>
-    <row r="22" spans="6:18" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F22" s="35" t="s">
         <v>75</v>
       </c>
@@ -2760,7 +2543,7 @@
       <c r="Q22" s="31"/>
       <c r="R22" s="31"/>
     </row>
-    <row r="23" spans="6:18" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F23" s="39"/>
       <c r="G23" s="40" t="s">
         <v>78</v>
@@ -2782,19 +2565,19 @@
       <c r="Q23" s="31"/>
       <c r="R23" s="31"/>
     </row>
-    <row r="24" spans="6:18" x14ac:dyDescent="0.35">
+    <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F24" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="10">
+      <c r="G24" s="10" t="n">
         <v>6050.78</v>
       </c>
-      <c r="H24" s="10">
+      <c r="H24" s="10" t="n">
         <v>69.91</v>
       </c>
-      <c r="I24" s="44">
-        <f>H24/$H$26*100</f>
-        <v>72.049881479954649</v>
+      <c r="I24" s="44" t="n">
+        <f aca="false">H24/$H$26*100</f>
+        <v>72.0498814799547</v>
       </c>
       <c r="M24" s="29"/>
       <c r="N24" s="29"/>
@@ -2803,68 +2586,76 @@
       <c r="Q24" s="31"/>
       <c r="R24" s="31"/>
     </row>
-    <row r="25" spans="6:18" x14ac:dyDescent="0.35">
+    <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F25" s="43"/>
-      <c r="G25" s="10">
+      <c r="G25" s="10" t="n">
         <v>6089.88</v>
       </c>
-      <c r="H25" s="10">
+      <c r="H25" s="10" t="n">
         <v>27.12</v>
       </c>
-      <c r="I25" s="44">
-        <f>H25/$H$26*100</f>
-        <v>27.950118520045347</v>
-      </c>
-    </row>
-    <row r="26" spans="6:18" x14ac:dyDescent="0.35">
+      <c r="I25" s="44" t="n">
+        <f aca="false">H25/$H$26*100</f>
+        <v>27.9501185200453</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F26" s="39"/>
       <c r="G26" s="40"/>
-      <c r="H26" s="40">
-        <f>SUM(H24:H25)</f>
+      <c r="H26" s="40" t="n">
+        <f aca="false">SUM(H24:H25)</f>
         <v>97.03</v>
       </c>
-      <c r="I26" s="44">
-        <f>SUM(I24:I25)</f>
+      <c r="I26" s="44" t="n">
+        <f aca="false">SUM(I24:I25)</f>
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="6:18" x14ac:dyDescent="0.35">
+    <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F27" s="45"/>
-      <c r="G27" s="46">
-        <f>(G24*I24+G25*I25)/100</f>
-        <v>6061.7084963413372</v>
+      <c r="G27" s="46" t="n">
+        <f aca="false">(G24*I24+G25*I25)/100</f>
+        <v>6061.70849634134</v>
       </c>
       <c r="H27" s="47"/>
       <c r="I27" s="48"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2:R6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="10" max="10" width="10" customWidth="1"/>
-    <col min="11" max="11" width="14.1796875" customWidth="1"/>
-    <col min="12" max="12" width="11.54296875" customWidth="1"/>
-    <col min="14" max="14" width="10.453125" customWidth="1"/>
-    <col min="16" max="16" width="8.1796875" customWidth="1"/>
-    <col min="18" max="18" width="10.26953125" customWidth="1"/>
-    <col min="19" max="19" width="10.7265625" customWidth="1"/>
-    <col min="20" max="20" width="9.6328125" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="8.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="10.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="10.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="9.63"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" customFormat="false" ht="29.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="49" t="s">
         <v>83</v>
       </c>
@@ -2911,430 +2702,435 @@
         <v>95</v>
       </c>
       <c r="S1" s="54" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="T1" s="54" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="55">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="55" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="56">
+      <c r="B2" s="56" t="n">
         <v>1910</v>
       </c>
-      <c r="C2" s="57">
+      <c r="C2" s="57" t="n">
         <v>1950</v>
       </c>
-      <c r="D2" s="58">
+      <c r="D2" s="58" t="n">
         <v>51254</v>
       </c>
-      <c r="E2" s="59">
+      <c r="E2" s="59" t="n">
         <v>45821.5</v>
       </c>
-      <c r="F2" s="58">
+      <c r="F2" s="58" t="n">
         <v>1936.37</v>
       </c>
-      <c r="G2" s="59">
+      <c r="G2" s="59" t="n">
         <v>1939</v>
       </c>
-      <c r="H2" s="58">
+      <c r="H2" s="58" t="n">
         <v>6.12</v>
       </c>
-      <c r="I2" s="59">
+      <c r="I2" s="59" t="n">
         <v>14.41</v>
       </c>
-      <c r="J2" s="60">
-        <f>H2*$K$9/1000</f>
-        <v>2.7429840000000004E-2</v>
-      </c>
-      <c r="K2" s="61">
-        <f>((H2*$K$10/1000)*2+($M$10/1000)*2)*0.5</f>
-        <v>8.1983360000000005E-2</v>
+      <c r="J2" s="60" t="n">
+        <f aca="false">H2*$K$9/1000</f>
+        <v>0.02742984</v>
+      </c>
+      <c r="K2" s="61" t="n">
+        <f aca="false">((H2*$K$10/1000)*2+($M$10/1000)*2)*0.5</f>
+        <v>0.08198336</v>
       </c>
       <c r="L2" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="M2" s="10">
-        <v>8784.3700000000008</v>
-      </c>
-      <c r="N2">
-        <f>F2*$K$9/1000+$M$9/1000</f>
-        <v>8.5736663400000008</v>
-      </c>
-      <c r="P2" s="62">
-        <f>$K$9*F2+$M$9</f>
-        <v>8573.6663399999998</v>
-      </c>
-      <c r="Q2" s="62">
-        <f>P2-M2</f>
-        <v>-210.70366000000104</v>
-      </c>
-      <c r="R2">
-        <f>K2/(M2/1000)</f>
-        <v>9.332867354175654E-3</v>
-      </c>
-      <c r="S2" s="63">
-        <f>J2/(M2/1000)</f>
-        <v>3.1225733888713704E-3</v>
-      </c>
-      <c r="T2" s="64">
-        <f>1/SQRT((M2/1000))</f>
-        <v>0.33739969833423611</v>
-      </c>
-      <c r="U2">
-        <f t="shared" ref="T2:U6" si="0">1/SQRT(N2)</f>
-        <v>0.3415204475574205</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="55">
+      <c r="M2" s="10" t="n">
+        <v>8784.37</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <f aca="false">F2*$K$9/1000+$M$9/1000</f>
+        <v>8.57366634</v>
+      </c>
+      <c r="P2" s="62" t="n">
+        <f aca="false">$K$9*F2+$M$9</f>
+        <v>8573.66634</v>
+      </c>
+      <c r="Q2" s="62" t="n">
+        <f aca="false">P2-M2</f>
+        <v>-210.703660000001</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <f aca="false">K2/(M2/1000)</f>
+        <v>0.00933286735417565</v>
+      </c>
+      <c r="S2" s="63" t="n">
+        <f aca="false">J2/(M2/1000)</f>
+        <v>0.00312257338887137</v>
+      </c>
+      <c r="T2" s="64" t="n">
+        <f aca="false">1/SQRT((M2/1000))</f>
+        <v>0.337399698334236</v>
+      </c>
+      <c r="U2" s="0" t="n">
+        <f aca="false">1/SQRT(N2)</f>
+        <v>0.34152044755742</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="55" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="56">
+      <c r="B3" s="56" t="n">
         <v>1460</v>
       </c>
-      <c r="C3" s="57">
+      <c r="C3" s="57" t="n">
         <v>1510</v>
       </c>
-      <c r="D3" s="58">
+      <c r="D3" s="58" t="n">
         <v>81328</v>
       </c>
-      <c r="E3" s="59">
+      <c r="E3" s="59" t="n">
         <v>78268</v>
       </c>
-      <c r="F3" s="58">
+      <c r="F3" s="58" t="n">
         <v>1488.93</v>
       </c>
-      <c r="G3" s="59">
+      <c r="G3" s="59" t="n">
         <v>1491</v>
       </c>
-      <c r="H3" s="58">
+      <c r="H3" s="58" t="n">
         <v>7.22</v>
       </c>
-      <c r="I3" s="59">
-        <v>17.010000000000002</v>
-      </c>
-      <c r="J3" s="60">
-        <f t="shared" ref="J3:J6" si="1">H3*$K$9/1000</f>
-        <v>3.236004E-2</v>
-      </c>
-      <c r="K3" s="61">
-        <f t="shared" ref="K3:K6" si="2">((H3*$K$10/1000)*2+($M$10/1000)*2)*0.5</f>
-        <v>8.2041660000000016E-2</v>
+      <c r="I3" s="59" t="n">
+        <v>17.01</v>
+      </c>
+      <c r="J3" s="60" t="n">
+        <f aca="false">H3*$K$9/1000</f>
+        <v>0.03236004</v>
+      </c>
+      <c r="K3" s="61" t="n">
+        <f aca="false">((H3*$K$10/1000)*2+($M$10/1000)*2)*0.5</f>
+        <v>0.08204166</v>
       </c>
       <c r="L3" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="M3" s="10">
+      <c r="M3" s="10" t="n">
         <v>6778.3</v>
       </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N6" si="3">F3*$K$9/1000+$M$9/1000</f>
-        <v>6.5682402600000005</v>
-      </c>
-      <c r="P3" s="62">
-        <f>$K$9*F3+$M$9</f>
-        <v>6568.2402600000005</v>
-      </c>
-      <c r="Q3" s="62">
-        <f>P3-M3</f>
-        <v>-210.05973999999969</v>
-      </c>
-      <c r="R3">
-        <f t="shared" ref="R3:R6" si="4">K3/(M3/1000)</f>
-        <v>1.2103574642609506E-2</v>
-      </c>
-      <c r="S3" s="63">
-        <f t="shared" ref="S3:S6" si="5">J3/(M3/1000)</f>
-        <v>4.7740642934069018E-3</v>
-      </c>
-      <c r="T3" s="64">
-        <f t="shared" ref="T3:T6" si="6">1/SQRT((M3/1000))</f>
-        <v>0.38409584294877042</v>
-      </c>
-      <c r="U3">
-        <f t="shared" si="0"/>
-        <v>0.39018941591302314</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="55">
+      <c r="N3" s="0" t="n">
+        <f aca="false">F3*$K$9/1000+$M$9/1000</f>
+        <v>6.56824026</v>
+      </c>
+      <c r="P3" s="62" t="n">
+        <f aca="false">$K$9*F3+$M$9</f>
+        <v>6568.24026</v>
+      </c>
+      <c r="Q3" s="62" t="n">
+        <f aca="false">P3-M3</f>
+        <v>-210.05974</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <f aca="false">K3/(M3/1000)</f>
+        <v>0.0121035746426095</v>
+      </c>
+      <c r="S3" s="63" t="n">
+        <f aca="false">J3/(M3/1000)</f>
+        <v>0.0047740642934069</v>
+      </c>
+      <c r="T3" s="64" t="n">
+        <f aca="false">1/SQRT((M3/1000))</f>
+        <v>0.38409584294877</v>
+      </c>
+      <c r="U3" s="0" t="n">
+        <f aca="false">1/SQRT(N3)</f>
+        <v>0.390189415913023</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="55" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="56">
+      <c r="B4" s="56" t="n">
         <v>1350</v>
       </c>
-      <c r="C4" s="57">
+      <c r="C4" s="57" t="n">
         <v>1400</v>
       </c>
-      <c r="D4" s="58">
+      <c r="D4" s="58" t="n">
         <v>82136</v>
       </c>
-      <c r="E4" s="59">
+      <c r="E4" s="59" t="n">
         <v>77903</v>
       </c>
-      <c r="F4" s="58">
+      <c r="F4" s="58" t="n">
         <v>1379.44</v>
       </c>
-      <c r="G4" s="59">
+      <c r="G4" s="59" t="n">
         <v>1383</v>
       </c>
-      <c r="H4" s="58">
+      <c r="H4" s="58" t="n">
         <v>7.32</v>
       </c>
-      <c r="I4" s="59">
-        <v>17.239999999999998</v>
-      </c>
-      <c r="J4" s="60">
-        <f t="shared" si="1"/>
-        <v>3.2808240000000002E-2</v>
-      </c>
-      <c r="K4" s="61">
-        <f t="shared" si="2"/>
-        <v>8.2046960000000016E-2</v>
+      <c r="I4" s="59" t="n">
+        <v>17.24</v>
+      </c>
+      <c r="J4" s="60" t="n">
+        <f aca="false">H4*$K$9/1000</f>
+        <v>0.03280824</v>
+      </c>
+      <c r="K4" s="61" t="n">
+        <f aca="false">((H4*$K$10/1000)*2+($M$10/1000)*2)*0.5</f>
+        <v>0.08204696</v>
       </c>
       <c r="L4" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="10" t="n">
         <v>6288.08</v>
       </c>
-      <c r="N4">
-        <f t="shared" si="3"/>
+      <c r="N4" s="0" t="n">
+        <f aca="false">F4*$K$9/1000+$M$9/1000</f>
         <v>6.07750608</v>
       </c>
-      <c r="P4" s="62">
-        <f>$K$9*F4+$M$9</f>
-        <v>6077.5060800000001</v>
-      </c>
-      <c r="Q4" s="62">
-        <f>P4-M4</f>
-        <v>-210.57391999999982</v>
-      </c>
-      <c r="R4">
-        <f t="shared" si="4"/>
-        <v>1.3048014656302086E-2</v>
-      </c>
-      <c r="S4" s="63">
-        <f t="shared" si="5"/>
-        <v>5.2175290390707504E-3</v>
-      </c>
-      <c r="T4" s="64">
-        <f t="shared" si="6"/>
-        <v>0.39878698020940273</v>
-      </c>
-      <c r="U4">
-        <f t="shared" si="0"/>
-        <v>0.40563675425566198</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="55">
+      <c r="P4" s="62" t="n">
+        <f aca="false">$K$9*F4+$M$9</f>
+        <v>6077.50608</v>
+      </c>
+      <c r="Q4" s="62" t="n">
+        <f aca="false">P4-M4</f>
+        <v>-210.57392</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <f aca="false">K4/(M4/1000)</f>
+        <v>0.0130480146563021</v>
+      </c>
+      <c r="S4" s="63" t="n">
+        <f aca="false">J4/(M4/1000)</f>
+        <v>0.00521752903907075</v>
+      </c>
+      <c r="T4" s="64" t="n">
+        <f aca="false">1/SQRT((M4/1000))</f>
+        <v>0.398786980209403</v>
+      </c>
+      <c r="U4" s="0" t="n">
+        <f aca="false">1/SQRT(N4)</f>
+        <v>0.405636754255662</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="55" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="56">
+      <c r="B5" s="56" t="n">
         <v>1310</v>
       </c>
-      <c r="C5" s="57">
+      <c r="C5" s="57" t="n">
         <v>1345</v>
       </c>
-      <c r="D5" s="58">
+      <c r="D5" s="58" t="n">
         <v>28227</v>
       </c>
-      <c r="E5" s="59">
+      <c r="E5" s="59" t="n">
         <v>19119</v>
       </c>
-      <c r="F5" s="58">
+      <c r="F5" s="58" t="n">
         <v>1328.67</v>
       </c>
-      <c r="G5" s="59">
+      <c r="G5" s="59" t="n">
         <v>1328</v>
       </c>
-      <c r="H5" s="58">
+      <c r="H5" s="58" t="n">
         <v>6.62</v>
       </c>
-      <c r="I5" s="59">
+      <c r="I5" s="59" t="n">
         <v>15.6</v>
       </c>
-      <c r="J5" s="60">
-        <f t="shared" si="1"/>
-        <v>2.967084E-2</v>
-      </c>
-      <c r="K5" s="61">
-        <f t="shared" si="2"/>
-        <v>8.2009860000000004E-2</v>
+      <c r="J5" s="60" t="n">
+        <f aca="false">H5*$K$9/1000</f>
+        <v>0.02967084</v>
+      </c>
+      <c r="K5" s="61" t="n">
+        <f aca="false">((H5*$K$10/1000)*2+($M$10/1000)*2)*0.5</f>
+        <v>0.08200986</v>
       </c>
       <c r="L5" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="M5" s="65">
-        <v>6061.7084963413399</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="3"/>
-        <v>5.8499549400000008</v>
-      </c>
-      <c r="P5" s="62">
-        <f>$K$9*F5+$M$9</f>
-        <v>5849.9549400000005</v>
-      </c>
-      <c r="Q5" s="62">
-        <f>P5-M5</f>
-        <v>-211.75355634133939</v>
-      </c>
-      <c r="R5">
-        <f t="shared" si="4"/>
-        <v>1.352916591906368E-2</v>
-      </c>
-      <c r="S5" s="63">
-        <f t="shared" si="5"/>
-        <v>4.8947982269204144E-3</v>
-      </c>
-      <c r="T5" s="64">
-        <f t="shared" si="6"/>
-        <v>0.40616498082144353</v>
-      </c>
-      <c r="U5">
-        <f t="shared" si="0"/>
-        <v>0.41345070761571706</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="55">
+      <c r="M5" s="65" t="n">
+        <v>6061.70849634134</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <f aca="false">F5*$K$9/1000+$M$9/1000</f>
+        <v>5.84995494</v>
+      </c>
+      <c r="P5" s="62" t="n">
+        <f aca="false">$K$9*F5+$M$9</f>
+        <v>5849.95494</v>
+      </c>
+      <c r="Q5" s="62" t="n">
+        <f aca="false">P5-M5</f>
+        <v>-211.753556341339</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <f aca="false">K5/(M5/1000)</f>
+        <v>0.0135291659190637</v>
+      </c>
+      <c r="S5" s="63" t="n">
+        <f aca="false">J5/(M5/1000)</f>
+        <v>0.00489479822692041</v>
+      </c>
+      <c r="T5" s="64" t="n">
+        <f aca="false">1/SQRT((M5/1000))</f>
+        <v>0.406164980821444</v>
+      </c>
+      <c r="U5" s="0" t="n">
+        <f aca="false">1/SQRT(N5)</f>
+        <v>0.413450707615717</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="55" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="56">
+      <c r="B6" s="56" t="n">
         <v>1220</v>
       </c>
-      <c r="C6" s="57">
+      <c r="C6" s="57" t="n">
         <v>1265</v>
       </c>
-      <c r="D6" s="58">
+      <c r="D6" s="58" t="n">
         <v>79587</v>
       </c>
-      <c r="E6" s="59">
+      <c r="E6" s="59" t="n">
         <v>72480</v>
       </c>
-      <c r="F6" s="58">
-        <v>1244.8399999999999</v>
-      </c>
-      <c r="G6" s="59">
+      <c r="F6" s="58" t="n">
+        <v>1244.84</v>
+      </c>
+      <c r="G6" s="59" t="n">
         <v>1246</v>
       </c>
-      <c r="H6" s="58">
+      <c r="H6" s="58" t="n">
         <v>7.31</v>
       </c>
-      <c r="I6" s="59">
+      <c r="I6" s="59" t="n">
         <v>17.21</v>
       </c>
-      <c r="J6" s="60">
-        <f t="shared" si="1"/>
-        <v>3.2763419999999994E-2</v>
-      </c>
-      <c r="K6" s="61">
-        <f t="shared" si="2"/>
-        <v>8.2046430000000004E-2</v>
+      <c r="J6" s="60" t="n">
+        <f aca="false">H6*$K$9/1000</f>
+        <v>0.03276342</v>
+      </c>
+      <c r="K6" s="61" t="n">
+        <f aca="false">((H6*$K$10/1000)*2+($M$10/1000)*2)*0.5</f>
+        <v>0.08204643</v>
       </c>
       <c r="L6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="M6" s="10">
+      <c r="M6" s="10" t="n">
         <v>5685.37</v>
       </c>
-      <c r="N6">
-        <f t="shared" si="3"/>
-        <v>5.4742288800000001</v>
-      </c>
-      <c r="P6" s="62">
-        <f>$K$9*F6+$M$9</f>
-        <v>5474.2288799999997</v>
-      </c>
-      <c r="Q6" s="62">
-        <f>P6-M6</f>
-        <v>-211.14112000000023</v>
-      </c>
-      <c r="R6">
-        <f t="shared" si="4"/>
-        <v>1.4431150479212436E-2</v>
-      </c>
-      <c r="S6" s="63">
-        <f t="shared" si="5"/>
-        <v>5.7627595037789969E-3</v>
-      </c>
-      <c r="T6" s="64">
-        <f t="shared" si="6"/>
-        <v>0.41939247443586286</v>
-      </c>
-      <c r="U6">
-        <f t="shared" si="0"/>
-        <v>0.42740394283589689</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="N6" s="0" t="n">
+        <f aca="false">F6*$K$9/1000+$M$9/1000</f>
+        <v>5.47422888</v>
+      </c>
+      <c r="P6" s="62" t="n">
+        <f aca="false">$K$9*F6+$M$9</f>
+        <v>5474.22888</v>
+      </c>
+      <c r="Q6" s="62" t="n">
+        <f aca="false">P6-M6</f>
+        <v>-211.14112</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <f aca="false">K6/(M6/1000)</f>
+        <v>0.0144311504792124</v>
+      </c>
+      <c r="S6" s="63" t="n">
+        <f aca="false">J6/(M6/1000)</f>
+        <v>0.005762759503779</v>
+      </c>
+      <c r="T6" s="64" t="n">
+        <f aca="false">1/SQRT((M6/1000))</f>
+        <v>0.419392474435863</v>
+      </c>
+      <c r="U6" s="0" t="n">
+        <f aca="false">1/SQRT(N6)</f>
+        <v>0.427403942835897</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J9" s="66" t="s">
-        <v>96</v>
-      </c>
-      <c r="K9" s="66">
-        <v>4.4820000000000002</v>
+        <v>98</v>
+      </c>
+      <c r="K9" s="66" t="n">
+        <v>4.482</v>
       </c>
       <c r="L9" s="66" t="s">
-        <v>97</v>
-      </c>
-      <c r="M9" s="66">
-        <v>-105.14400000000001</v>
-      </c>
-      <c r="O9" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+      <c r="M9" s="66" t="n">
+        <v>-105.144</v>
+      </c>
+      <c r="O9" s="0" t="s">
+        <v>100</v>
       </c>
       <c r="R9" s="67" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="68" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C10" s="68" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D10" s="68" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J10" s="69" t="s">
-        <v>103</v>
-      </c>
-      <c r="K10">
-        <v>5.2999999999999999E-2</v>
+        <v>105</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>0.053</v>
       </c>
       <c r="L10" s="69" t="s">
-        <v>103</v>
-      </c>
-      <c r="M10">
-        <v>81.659000000000006</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>81.659</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J12" s="70" t="s">
-        <v>104</v>
-      </c>
-      <c r="K12" s="70">
+        <v>106</v>
+      </c>
+      <c r="K12" s="70" t="n">
         <v>0.2989</v>
       </c>
       <c r="L12" s="70" t="s">
-        <v>105</v>
-      </c>
-      <c r="M12" s="70">
-        <v>-1.6000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="13:13" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+      <c r="M12" s="70" t="n">
+        <v>-0.0016</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M17" s="71"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>